<commit_message>
20250401 WIFRP almost done
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202503/SESAMm.xlsx
+++ b/GUI + Reviews/202503/SESAMm.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202503\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202503/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B525B5-D652-4ECC-BCAB-EE1DD1EAD3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{40B525B5-D652-4ECC-BCAB-EE1DD1EAD3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{507B6783-5931-47AE-910D-FC8FB3402726}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-315" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$335</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2455,7 +2455,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8768,6 +8770,7 @@
       <c r="E361" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F335" xr:uid="{8BBBED01-1B80-4FBF-8E05-AE91AA70AE60}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFFEF00 PRIVATE</oddFooter>

</xml_diff>